<commit_message>
Completed GUI for all Entities
All objects in the world are now initialised sensibly within the grid
world and rendered nicely.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -53,7 +53,7 @@
     <t>Updated journal and created the timesheet. So few public data points on how long things actually take made me decide to track this better and make it public. Added some methods to world state class. Sorted out the graphics to display grid and adventurer.</t>
   </si>
   <si>
-    <t>Added Wumpus and stenches in addition to Adventurer. Renders well, simplify the iconography so I can just use core drawing functions. Solid ovals for things, empty ovals for their signals. Must update documention.</t>
+    <t>Added Wumpus and stenches in addition to Adventurer. Renders well, simplify the iconography so I can just use core drawing functions. Solid ovals for things, empty ovals for their signals. Must update documention. Got the rest of the images drawn for the pits, breezes, gold and glitter. Need to turn of the random seed as we get no variation in runs.</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -500,7 +500,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>34</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -597,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>42899</v>
       </c>
@@ -606,7 +606,7 @@
         <v>42899</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Implemented the random action brain
Agent chooses an action at random. This will be what the other
algorithms are compared agains.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -53,7 +53,7 @@
     <t>Updated journal and created the timesheet. So few public data points on how long things actually take made me decide to track this better and make it public. Added some methods to world state class. Sorted out the graphics to display grid and adventurer.</t>
   </si>
   <si>
-    <t>Added Wumpus and stenches in addition to Adventurer. Renders well, simplify the iconography so I can just use core drawing functions. Solid ovals for things, empty ovals for their signals. Must update documention. Got the rest of the images drawn for the pits, breezes, gold and glitter. Need to turn of the random seed as we get no variation in runs.</t>
+    <t>Added Wumpus and stenches in addition to Adventurer. Renders well, simplify the iconography so I can just use core drawing functions. Solid ovals for things, empty ovals for their signals. Must update documention. Got the rest of the images drawn for the pits, breezes, gold and glitter. Need to turn of the random seed as we get no variation in runs. Created the Adventurer Agent class that initially moves randomly.</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -500,7 +500,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>37.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -597,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>42899</v>
       </c>
@@ -606,7 +606,7 @@
         <v>42899</v>
       </c>
       <c r="C9" s="1">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added properties file handling.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -59,7 +59,10 @@
     <t>Created the Adventurer Agent class that initially moves randomly.</t>
   </si>
   <si>
-    <t>Defined the first draft of the data model for reporting work package.</t>
+    <t>Defined the first draft of the data model for reporting work package and started building the properties file handling.</t>
+  </si>
+  <si>
+    <t>fleshed out the properties handling.</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -506,7 +509,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>39.5</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -633,7 +636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>42901</v>
       </c>
@@ -642,10 +645,25 @@
         <v>42901</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="5">
+        <v>42902</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" ref="B12" si="4">A12</f>
+        <v>42902</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished integrating properties file.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>fleshed out the properties handling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished integrating the properties file into the code base. Introduced some errors along the way that took a while to fix. Also changed glitter to appear only in the cell with the gold in keeping with the standard wumpus world model. </t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -509,7 +512,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>41.5</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -656,7 +659,7 @@
         <v>42902</v>
       </c>
       <c r="B12" s="4">
-        <f t="shared" ref="B12" si="4">A12</f>
+        <f t="shared" ref="B12:B13" si="4">A12</f>
         <v>42902</v>
       </c>
       <c r="C12" s="1">
@@ -664,6 +667,21 @@
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A13" s="5">
+        <v>42904</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="4"/>
+        <v>42904</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed the data logger for experiment data.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t xml:space="preserve">Finished integrating the properties file into the code base. Introduced some errors along the way that took a while to fix. Also changed glitter to appear only in the cell with the gold in keeping with the standard wumpus world model. </t>
+  </si>
+  <si>
+    <t>Working on logging function. Running 100 simulations with random behaviour to generate log of base case.</t>
+  </si>
+  <si>
+    <t>Created a spreadsheet to analyse baseline data, found a bug in simulator from the statistical data. Fixed simulator and generated another data set.</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -512,7 +518,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>45.5</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -682,6 +688,36 @@
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="5">
+        <v>42905</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" ref="B14" si="5">A14</f>
+        <v>42905</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="5">
+        <v>42906</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" ref="B15" si="6">A15</f>
+        <v>42906</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logging and analysis finished
For this iteration logging and analysis is completed. Have baseline data
based on random actions to compare q learning against.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -71,7 +71,7 @@
     <t>Working on logging function. Running 100 simulations with random behaviour to generate log of base case.</t>
   </si>
   <si>
-    <t>Created a spreadsheet to analyse baseline data, found a bug in simulator from the statistical data. Fixed simulator and generated another data set.</t>
+    <t>Created a spreadsheet to analyse baseline data, found a bug in simulator from the statistical data. Fixed simulator and generated another data set. Logging and reporting is finished for this iteration.</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -518,7 +518,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>49.5</v>
+        <v>50.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -705,7 +705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>42906</v>
       </c>
@@ -714,7 +714,7 @@
         <v>42906</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Released under apache 2
Change licencing to apache 2 licence.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>q brain. This took far longer than I expected. Many dead ends, design changes, rabbit holes. Finally realized it was much simpler than I thought and with much angst I stripped out dozens of lines of code simplifying it. It now works as expected but I've somehow broken the GUI.</t>
+  </si>
+  <si>
+    <t>Put in the basic structure for a menu, with File, Edit and Run. Discovered Java doesn’t cope with high dpi displays without manually setting font sizes.</t>
+  </si>
+  <si>
+    <t>Added breeze and stench feedback into the learning algorith and ran some experiments to guage impact. Have to reward exploration otherwise Adventurer dies of starvation.</t>
   </si>
 </sst>
 </file>
@@ -478,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -527,7 +533,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>79.5</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -749,7 +755,7 @@
         <v>42908</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" ref="B17:B21" si="8">A17</f>
+        <f t="shared" ref="B17:B23" si="8">A17</f>
         <v>42908</v>
       </c>
       <c r="C17" s="1">
@@ -817,6 +823,36 @@
       </c>
       <c r="D21" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="5">
+        <v>42917</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="8"/>
+        <v>42917</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="5">
+        <v>42918</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" si="8"/>
+        <v>42918</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the colour update to the QStateViewer. There appears to be a defect in the comparison function of doubles where all the values are negative. I implemented a simple rescaling operation and it all displays perfectly.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Partially retired the logging function that reported the q values. Willl likelly delete the code during a later refactoring.</t>
+  </si>
+  <si>
+    <t>Started using the FileChooser class to open configuration files and the text is too small to read. I can't fix this the way I have with the other gui components. Looks like I have to convert the entire application to JavaFX.</t>
   </si>
 </sst>
 </file>
@@ -502,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -551,7 +554,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -957,6 +960,21 @@
       </c>
       <c r="D29" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A30" s="5">
+        <v>42938</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30" si="11">A30</f>
+        <v>42938</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support to get properties file from the command line when WWS is launched. This means we can create a series of simulations using different property file and run them from the command line rather than from the IDE or mmanually changing the files each timee.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Started using the FileChooser class to open configuration files and the text is too small to read. I can't fix this the way I have with the other gui components. Looks like I have to convert the entire application to JavaFX.</t>
+  </si>
+  <si>
+    <t>Built an executable Jar file, cleaned up the q state viewer colour coding, there may be a bug in how Java handles irrational negative doubles, learnt how to make a youtube video and published my first video on youtube.</t>
   </si>
 </sst>
 </file>
@@ -505,9 +508,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -554,7 +557,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -967,7 +970,7 @@
         <v>42938</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" ref="B30" si="11">A30</f>
+        <f t="shared" ref="B30:B31" si="11">A30</f>
         <v>42938</v>
       </c>
       <c r="C30" s="1">
@@ -975,6 +978,21 @@
       </c>
       <c r="D30" s="2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A31" s="5">
+        <v>42946</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="11"/>
+        <v>42946</v>
+      </c>
+      <c r="C31" s="1">
+        <v>7</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement junit testing. Immplement persistance of the brain state.
</commit_message>
<xml_diff>
--- a/Spreadsheets/TimeSpent.xlsx
+++ b/Spreadsheets/TimeSpent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Built an executable Jar file, cleaned up the q state viewer colour coding, there may be a bug in how Java handles irrational negative doubles, learnt how to make a youtube video and published my first video on youtube.</t>
+  </si>
+  <si>
+    <t>Adding test cases and persistance to QTableBrain.</t>
+  </si>
+  <si>
+    <t>debugging persistance.</t>
+  </si>
+  <si>
+    <t>Refactored the choosing of random locations so always guaranteed to be in an empty cell.</t>
   </si>
 </sst>
 </file>
@@ -508,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -557,7 +566,7 @@
       </c>
       <c r="F2" s="1">
         <f>SUM(C:C)</f>
-        <v>106</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -970,7 +979,7 @@
         <v>42938</v>
       </c>
       <c r="B30" s="4">
-        <f t="shared" ref="B30:B31" si="11">A30</f>
+        <f t="shared" ref="B30:B32" si="11">A30</f>
         <v>42938</v>
       </c>
       <c r="C30" s="1">
@@ -993,6 +1002,51 @@
       </c>
       <c r="D31" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="5">
+        <v>42953</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="11"/>
+        <v>42953</v>
+      </c>
+      <c r="C32" s="1">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="5">
+        <v>42954</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" ref="B33" si="12">A33</f>
+        <v>42954</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="5">
+        <v>42955</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" ref="B34" si="13">A34</f>
+        <v>42955</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>